<commit_message>
docs: addcontent to README.md file
</commit_message>
<xml_diff>
--- a/externals/testCases.xlsx
+++ b/externals/testCases.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="62">
   <si>
     <t xml:space="preserve">TestSteps</t>
   </si>
@@ -157,6 +157,60 @@
   </si>
   <si>
     <t xml:space="preserve">Keyword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">baseUrl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">startingPopUp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">singleResult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multipleCheck4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tuesday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thursday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">friday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saturday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sunday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">radio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">radiobutton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">radioResult</t>
   </si>
 </sst>
 </file>
@@ -282,7 +336,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -763,7 +817,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -828,15 +882,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="65.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -852,9 +907,190 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>